<commit_message>
Updated commissioning_template.xlsx to reflect new AQUA roles
</commit_message>
<xml_diff>
--- a/commissioning_template.xlsx
+++ b/commissioning_template.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CA3C13-39B1-4C8A-BB0D-8CB22F06E5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F0E02C-2591-40D9-8FC2-B1C2291D5D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36936" yWindow="2520" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29385" yWindow="645" windowWidth="27810" windowHeight="15315" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
   <si>
     <t>If there are concerns or ideas that are not addressed, please email the owner at  (EMAIL)</t>
   </si>
@@ -114,15 +114,6 @@
     <t>Ended on (date)</t>
   </si>
   <si>
-    <t>Have you reviewed the relevantresponsibilites of your role found in the sheet 'R&amp;R Resources'?</t>
-  </si>
-  <si>
-    <t>Do you agree to uphold the roles and responsibilties outlined in the sheet 'R&amp;R Resources'?</t>
-  </si>
-  <si>
-    <t>Please record here which documents you have created to evidence your work in your role</t>
-  </si>
-  <si>
     <t>Date of last review/update</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>Next review/update due on</t>
   </si>
   <si>
-    <t>SRO</t>
-  </si>
-  <si>
     <t>Commissioner</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>Analytical Assurer Overview</t>
   </si>
   <si>
-    <t>Commisioner Responsibilites</t>
-  </si>
-  <si>
     <t>Analytical Assurer Responsibilites</t>
   </si>
   <si>
@@ -172,18 +157,6 @@
   </si>
   <si>
     <t>I agree to ensure a high level of understanding of the requirements, scope and context of the analysis, not just for myself, but for the SRO, the Analytical Assurer and the Analyst(s)</t>
-  </si>
-  <si>
-    <t>I agree to quantify input error, major assumptions, limitations and uncertainty mathematically wherever possible.</t>
-  </si>
-  <si>
-    <t>I will ensure that the feedback given by the Quality Assurers is fully documented and reviewed by the modelling team</t>
-  </si>
-  <si>
-    <t>I agree to honestly and openly communicate errors in the model before and after publication to the end users. In particular, if an error is detected post publication, I agree to not withhold information regarding the error from the public and the end users.</t>
-  </si>
-  <si>
-    <t>SRO Documents</t>
   </si>
   <si>
     <t>Commissioner Documents</t>
@@ -235,177 +208,19 @@
     </r>
   </si>
   <si>
-    <t>Senior Responsible Owner overview</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The Senior Responsible Owner (SRO) owns the analysis. It is the SRO's responsibility to ensure the documentation here is kept up to date and is signed off </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>by them</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">. They act as the final decision maker on analysis design choices, liasing with the Commissoner if the decisions are very complex or difficult. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>They should make sure that these decisions are documented</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">. It is their responsibility to make sure that the limitations, uncertainties and assumptions of the analysis are sufficiently communicated to users of the final product. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>The commissioner acts as the liason between the end user and the analytical team. They ensure that the analysis is designed according to the end user need. This means transmitting needs from end users to analysts and concerns and limitations from analysts to end users.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> The flow of information should be two-way.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>The analytical assurer makes sure that sufficient and appropriate quality assurance</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> is planned and occurs during analysis development</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">. Quality assurance </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>should happen throughout, and not just at the end of development</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>. Most often this involves setting out a clear quality assurance plan, identifying quality assurers and peer review, scheduling time into the development to allow them to work and ensuring that their feedback is reviewed and implemented into the analysis, where appropriate.</t>
-    </r>
-  </si>
-  <si>
     <t>I agree to review and sign off all key decisions made about the analysis</t>
   </si>
   <si>
     <t>I agree to ensure that sufficent quality assurance happens throughout analysis development and that the analysis complies with the ONS Quality Standard for Analysis</t>
   </si>
   <si>
-    <t>I agree to communicate key risks, limitations, major assumptions of the analysis and uncertainty associated with the outcomes to users</t>
-  </si>
-  <si>
-    <t>I agree to ensure that quality assurance is sufficiently varied, including code review, documentation review, methodological review and discussion with the analysis team to ensure development occurs as planned.</t>
-  </si>
-  <si>
     <t>I agree to understand and keep up to date with the the strengths, limitations and contexts of the analysis</t>
   </si>
   <si>
-    <t>I agree to attempt to mittigate assumptions and limitations by improving analysis design wherever possible.</t>
-  </si>
-  <si>
     <t>I agree to remain up to date and informed of uncertainties in the analysis and their implications </t>
   </si>
   <si>
-    <t>I agree to ensure that relevant limitations, uncertainties and caveats detected by quality assurance are communicated to end users, both before and after publication.</t>
-  </si>
-  <si>
-    <t>I agree to ensure that the quality assurance process is compliant and appropriate, documenting findings and reviewing them to inform future analysis development.</t>
-  </si>
-  <si>
-    <t>I agree to transmit information regarding the strengths, limitations, context and uncertainties from the analytical team to end users to ensure appropriate analysis development.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">I agree to communicate the concerns of my analysis team to the commissioner. These concerns can include quality, timeline and feasability concerns. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>It is not acceptable for me to ignore the concerns of the analysis team.</t>
-    </r>
-  </si>
-  <si>
     <t>I agree to transmit information regarding user needs from end users to the analysis team, ensuring that the analysis is developed according to user needs</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Commissioning document: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Sets out the question the analysis tries to answer and how this analysis will try to answer it. The commissioning document must be completed before production begins. It should be created in collaboration with end users and the analytical team. The document must set out broad specifications for the analysis including accuracy requirements, delivery timeline and skill gaps that must be addressed before completion.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>QA Plan &amp; Log:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Sets out the planned quality assurance which should occur before the publication of the analysis. It must include a broad outline of the types of review that will occur (e.g. code review, documentation review, external peer review) as well as indicative dates for when the reviews will occur and who will perform them. Peer reviewers should be contacted well in advance of the start date of the review. The required time, resources and documentation should be discussed with them well in advance of the start date.</t>
-    </r>
   </si>
   <si>
     <t>Senior Responsible Owner</t>
@@ -612,12 +427,160 @@
   <si>
     <t>While most of the template should be self explanatory, this introductory slide sets out basic guidance on use.</t>
   </si>
+  <si>
+    <t>AQUA Book Roles in Analysis</t>
+  </si>
+  <si>
+    <t>Approver (Senior Responsible Owner) overview</t>
+  </si>
+  <si>
+    <t>The approver (may be known as senior analyst or senior responsible officer):
+scrutinises the work of the analyst and assurer
+confirms (if necessary) to the analyst, assurer and commissioner that the work has been appropriately assured</t>
+  </si>
+  <si>
+    <t>The commissioner:
+requests the analysis and sets out their requirements
+agrees that what the analyst is going to do will satisfy the need
+accepts the analysis and assurance as fit for purpose</t>
+  </si>
+  <si>
+    <t>The analytical assurer:
+reviews the assurance completed by the analyst
+carries out any further validation and verification they may see as appropriate
+reports errors and areas for improvement to the analyst
+undertakes repeated reviews as required
+confirms the work has been appropriately scoped, executed, validated and verified and documented to the approver
+can be a group of assurers, in which case the leader of the group is responsible
+must be independent from the analysts</t>
+  </si>
+  <si>
+    <t>Analyst Overview</t>
+  </si>
+  <si>
+    <t>The analyst:
+designs the approach, including the assurance, to meet the commissioner’s requirements
+agrees the approach with the commissioner
+carries out the analysis
+carries out their own assurance
+acts on findings from the assurer
+can be a group of analysts, in which case the lead analyst is responsible</t>
+  </si>
+  <si>
+    <t>Approver (SRO)</t>
+  </si>
+  <si>
+    <t>Commissioner Responsibilites</t>
+  </si>
+  <si>
+    <t>Analyst Responsibilities</t>
+  </si>
+  <si>
+    <t>I agree to design the analysis and assurance in line with commissioned requirements and ensure that the design complies with the ONS Quality Standard for Analysis</t>
+  </si>
+  <si>
+    <t>I agree to ensure tha key risks, limitations, major assumptions of the analysis and uncertainty associated with the outcomes are communicated appropriately to users</t>
+  </si>
+  <si>
+    <t>I agree to ensure that quality assurance is appropriately varied, including code review, documentation review, methodological review and discussion with the analysis team when required to ensure development occurs as planned.</t>
+  </si>
+  <si>
+    <t>I agree to set up sufficent quality assurance throughout the analysis and to ensure that the analysis complies with the ONS Quality Standard for Analysis</t>
+  </si>
+  <si>
+    <t>I agree to ensure that the analysis quantifies input error, major assumptions, limitations and uncertainty mathematically wherever possible.</t>
+  </si>
+  <si>
+    <t>I will ensure that the feedback given by the Quality Assurers is fully documented and reviewed by the analysts</t>
+  </si>
+  <si>
+    <t>I agree to ensure that the analysis is appropriately documented in line with the ONS Quality Standard for Analysis.</t>
+  </si>
+  <si>
+    <t>I agree to improve analysis design wherever possible.</t>
+  </si>
+  <si>
+    <t>I agree to ensure that relevant limitations, uncertainties and caveats detected by quality assurance are communicated to end users appropriately by the analytical team.</t>
+  </si>
+  <si>
+    <t>I will ensure that the feedback given by the Quality Assurers is fully considered and taken on board by the analyst team</t>
+  </si>
+  <si>
+    <t>I agree to ensure that quality assurance complies with the ONS Quality Standard for Analysis, documenting findings and reviewing them to inform future analysis development.</t>
+  </si>
+  <si>
+    <t>I agree to transmit information regarding the strengths, limitations, context and uncertainties from the analytical team to end users as appropriate to ensure appropriate analysis development.</t>
+  </si>
+  <si>
+    <t>I agree to ensure that relevant assumptions, limitations, uncertainties and caveats are communicated to end users appropriately by the analytical team.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I agree to communicate concerns of the analysis team to the commissioner where these will have a material impact on delivery. These concerns can include quality, timeline and feasibility concerns. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>It is not acceptable to ignore the concerns of the analysis team.</t>
+    </r>
+  </si>
+  <si>
+    <t>Approver Documents</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Commissioning document: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Sets out the question the analysis tries to answer and how this analysis will try to answer it. 
+The commissioning document must be completed before production begins. It should be created in collaboration with end users and the analytical team. The document must set out broad specifications for the analysis including accuracy requirements, delivery timeline and skill gaps that must be addressed before completion.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>QA Plan &amp; Log:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Sets out the planned quality assurance which should occur before the publication of the analysis. 
+It must include a broad outline of the types of review that will occur (e.g. code review, documentation review, external peer review) as well as indicative dates for when the reviews will occur and who will perform them. 
+Peer reviewers should be contacted well in advance of the start date of the review. The required time, resources and documentation should be discussed with them well in advance of the start date.</t>
+    </r>
+  </si>
+  <si>
+    <t>Have you reviewed the responsibilites of your role from the sheet 'R&amp;R Resources'?</t>
+  </si>
+  <si>
+    <t>Do you agree to undertake the roles and responsibilties outlined in the sheet 'R&amp;R Resources'?</t>
+  </si>
+  <si>
+    <t>Please link here the documents you have created to evidence your work in your role</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Ethical issues relating to the analysis should be considered and documented.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +711,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -948,7 +925,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1023,9 +1000,6 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1035,12 +1009,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1070,45 +1038,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1139,6 +1074,75 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1909,40 +1913,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0E718D-ABA6-478B-BFB8-19647D312746}">
   <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="17"/>
-    <col min="2" max="2" width="15.77734375" style="52" customWidth="1"/>
-    <col min="3" max="3" width="94.21875" style="24" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="17"/>
+    <col min="2" max="2" width="15.7109375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="94.28515625" style="24" customWidth="1"/>
     <col min="4" max="4" width="39" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="9.21875" style="17"/>
+    <col min="5" max="16384" width="9.28515625" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="53" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="53" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="67" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="50" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="53" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="50" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="28" t="s">
         <v>2</v>
       </c>
@@ -1950,69 +1954,73 @@
         <v>3</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="51"/>
-    </row>
-    <row r="9" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="51" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="51"/>
-    </row>
-    <row r="10" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="51"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" s="24"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15" s="24"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D16" s="24"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2027,94 +2035,94 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="17"/>
-    <col min="2" max="2" width="23.5546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="72.77734375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="97.44140625" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="9.21875" style="17"/>
+    <col min="1" max="1" width="9.28515625" style="17"/>
+    <col min="2" max="2" width="23.5703125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="72.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.42578125" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="9.28515625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C2" s="21"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C3" s="22"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C4" s="22"/>
     </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="20"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="19"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="23"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="28" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="28" t="s">
         <v>12</v>
       </c>
@@ -2123,65 +2131,65 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="22"/>
-      <c r="D19" s="71" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="26" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C20" s="22"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="20"/>
-      <c r="D21" s="71" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="25"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="20"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C25" s="22"/>
     </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="28" t="s">
         <v>20</v>
       </c>
@@ -2193,6 +2201,10 @@
     <hyperlink ref="D19" r:id="rId2" xr:uid="{DCB5EAF3-7ABD-4E22-AD36-913393C17FF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2207,180 +2219,184 @@
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="17"/>
-    <col min="2" max="2" width="23.5546875" style="49" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" style="17"/>
-    <col min="6" max="6" width="24.77734375" style="24" customWidth="1"/>
-    <col min="7" max="16384" width="9.21875" style="17"/>
+    <col min="1" max="1" width="9.28515625" style="17"/>
+    <col min="2" max="2" width="23.5703125" style="46" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="17"/>
+    <col min="6" max="6" width="24.7109375" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.28515625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="48"/>
-    </row>
-    <row r="2" spans="1:8" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="72" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="46"/>
-      <c r="F2" s="50"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="45"/>
+    </row>
+    <row r="2" spans="1:8" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43"/>
+      <c r="B2" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="59" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="43"/>
+      <c r="F8" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="59"/>
+      <c r="F13" s="17"/>
+      <c r="H13" s="65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="59"/>
+      <c r="F14" s="17"/>
+      <c r="H14" s="65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="H15" s="65"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="66"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="62" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="D17" s="66"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="59"/>
+      <c r="D18" s="66"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="59"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="59"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="73" t="s">
+      <c r="B21" s="59" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="74" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="75" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="76" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="78" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="79" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="73"/>
-      <c r="F13" s="17"/>
-      <c r="H13" s="79" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="73"/>
-      <c r="F14" s="17"/>
-      <c r="H14" s="79" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="75" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="H15" s="79"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="80"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="D17" s="80"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="73"/>
-      <c r="D18" s="80"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="73"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="73"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="73" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="73" t="s">
-        <v>122</v>
-      </c>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="73"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="59"/>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -2390,36 +2406,36 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A10" sqref="A10:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1"/>
-    <col min="2" max="2" width="29.33203125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="16.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.21875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="1"/>
+    <col min="2" max="2" width="29.28515625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -2430,7 +2446,7 @@
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2443,59 +2459,59 @@
       <c r="J3" s="8"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2508,12 +2524,12 @@
       <c r="J8" s="8"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
@@ -2524,28 +2540,28 @@
         <v>23</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="15" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -2557,10 +2573,10 @@
       <c r="J11" s="9"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -2572,9 +2588,9 @@
       <c r="J12" s="10"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -2585,30 +2601,30 @@
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2617,32 +2633,62 @@
       <c r="G17" s="6"/>
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B4:G7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11:G14 G16:G18" xr:uid="{C8DFCC39-3213-4086-86D5-016C311A6566}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11:G15 G17:G19" xr:uid="{044BCEB0-C1B1-4181-BBF3-04162C6044CC}">
       <formula1>"Resolved, Shelved"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2651,416 +2697,322 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:S1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="61" customWidth="1"/>
-    <col min="2" max="2" width="103.21875" style="61" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="61" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.21875" style="61"/>
-    <col min="6" max="6" width="30" style="61" customWidth="1"/>
-    <col min="7" max="7" width="71.5546875" style="62" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="61" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.21875" style="61"/>
-    <col min="11" max="11" width="30" style="61" customWidth="1"/>
-    <col min="12" max="12" width="97.5546875" style="61" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="61" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.21875" style="61"/>
+    <col min="1" max="1" width="18.85546875" style="34" customWidth="1"/>
+    <col min="2" max="2" width="74.42578125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="34"/>
+    <col min="6" max="6" width="30" style="34" customWidth="1"/>
+    <col min="7" max="7" width="71.5703125" style="31" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="34"/>
+    <col min="11" max="11" width="30" style="34" customWidth="1"/>
+    <col min="12" max="12" width="97.5703125" style="34" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="34"/>
+    <col min="16" max="16" width="24.85546875" style="34" customWidth="1"/>
+    <col min="17" max="17" width="56.7109375" style="34" customWidth="1"/>
+    <col min="18" max="18" width="14" style="34" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="34"/>
+    <col min="20" max="16384" width="9.28515625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="78" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="P4" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q4" s="80" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="37"/>
+      <c r="K5" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-    </row>
-    <row r="4" spans="1:14" ht="69" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="66" t="s">
+      <c r="C6" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="36" t="s">
+      <c r="D6" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="44" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" s="38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="84" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="G7" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="37" t="s">
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="L7" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="Q7" s="86" t="s">
+        <v>117</v>
+      </c>
+      <c r="R7" s="87"/>
+      <c r="S7" s="40"/>
+    </row>
+    <row r="8" spans="1:19" s="53" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-    </row>
-    <row r="8" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="39" t="s">
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+    </row>
+    <row r="9" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="84" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="G9" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="L9" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="Q9" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+    </row>
+    <row r="10" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="84" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="G10" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="L10" s="85" t="s">
+        <v>125</v>
+      </c>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="Q10" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+    </row>
+    <row r="11" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="84" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="G11" s="90" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="Q11" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+    </row>
+    <row r="12" spans="1:19" ht="58.5" x14ac:dyDescent="0.2">
+      <c r="B12" s="91" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="G12" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="K14" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="39" t="s">
+    </row>
+    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="G15" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="68" t="s">
+      <c r="H15" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-    </row>
-    <row r="10" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="42" t="s">
+      <c r="I15" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-    </row>
-    <row r="11" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="32" t="s">
+      <c r="M15" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="129" x14ac:dyDescent="0.2">
+      <c r="G16" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-    </row>
-    <row r="12" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-    </row>
-    <row r="13" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-    </row>
-    <row r="14" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="M17" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="N17" s="39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="34"/>
-      <c r="L18" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
+      <c r="L16" s="92" t="s">
+        <v>133</v>
+      </c>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3069,27 +3021,32 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="B2:B4"/>
+  <dimension ref="B1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3097,16 +3054,17 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{F0927FC3-1838-4B9C-A65A-AFE56E621375}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;K000000 OFFICIAL-FOR PUBLIC RELEASE</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3289,15 +3247,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3322,10 +3284,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{9ff2627b-e365-4c50-8f1e-0699f40c3c6e}" enabled="1" method="Privileged" siteId="{078807bf-ce82-4688-bce0-0d811684dc46}" contentBits="3" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>